<commit_message>
Updated car ownership targets based on 2035_TM152_FBP_Plus_20_AV0
</commit_message>
<xml_diff>
--- a/utilities/RTP/QAQC/Car_ownership_summary_2035.xlsx
+++ b/utilities/RTP/QAQC/Car_ownership_summary_2035.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\RTP2021\Blueprint\2035_TM152_FBP_Plus_10\OUTPUT\QAQC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\RTP2021\Blueprint\2035_TM152_FBP_Plus_20\OUTPUT\QAQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FBC48D-6C27-4056-BEF7-C420EC55FE55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11070"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="366" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,17 +18,26 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$13</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>nAVs</t>
   </si>
@@ -131,19 +141,30 @@
     <t>Car ownership level for the upper nest</t>
   </si>
   <si>
-    <t>Blueprint 2035 - target nhhld</t>
-  </si>
-  <si>
-    <t>Blueprint 2035 - target share</t>
-  </si>
-  <si>
     <t>shifts</t>
+  </si>
+  <si>
+    <t>Targets</t>
+  </si>
+  <si>
+    <t>Blueprint 2035 - no AV nhhld
+2035_TM152_FBP_Plus_20_AV0</t>
+  </si>
+  <si>
+    <t>Blueprint 2035 - no AV share
+2035_TM152_FBP_Plus_20_AV0</t>
+  </si>
+  <si>
+    <t>Model run</t>
+  </si>
+  <si>
+    <t>Target share</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -272,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -301,7 +322,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -328,15 +348,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent 2" xfId="1"/>
+    <cellStyle name="Percent 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -363,7 +385,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -641,341 +663,349 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.46484375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" style="8"/>
-    <col min="3" max="3" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.265625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="28" customWidth="1"/>
-    <col min="6" max="7" width="10.59765625" style="8" customWidth="1"/>
-    <col min="8" max="9" width="10.73046875" style="9" customWidth="1"/>
-    <col min="10" max="197" width="9.06640625" style="8"/>
-    <col min="198" max="198" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="10.59765625" style="8" customWidth="1"/>
-    <col min="201" max="215" width="10.73046875" style="8" customWidth="1"/>
-    <col min="216" max="453" width="9.06640625" style="8"/>
-    <col min="454" max="454" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="455" max="455" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="456" max="456" width="10.59765625" style="8" customWidth="1"/>
-    <col min="457" max="471" width="10.73046875" style="8" customWidth="1"/>
-    <col min="472" max="709" width="9.06640625" style="8"/>
-    <col min="710" max="710" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="711" max="711" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="712" max="712" width="10.59765625" style="8" customWidth="1"/>
-    <col min="713" max="727" width="10.73046875" style="8" customWidth="1"/>
-    <col min="728" max="965" width="9.06640625" style="8"/>
-    <col min="966" max="966" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="967" max="967" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="968" max="968" width="10.59765625" style="8" customWidth="1"/>
-    <col min="969" max="983" width="10.73046875" style="8" customWidth="1"/>
-    <col min="984" max="1221" width="9.06640625" style="8"/>
-    <col min="1222" max="1222" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="1223" max="1223" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1224" max="1224" width="10.59765625" style="8" customWidth="1"/>
-    <col min="1225" max="1239" width="10.73046875" style="8" customWidth="1"/>
-    <col min="1240" max="1477" width="9.06640625" style="8"/>
-    <col min="1478" max="1478" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="1479" max="1479" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1480" max="1480" width="10.59765625" style="8" customWidth="1"/>
-    <col min="1481" max="1495" width="10.73046875" style="8" customWidth="1"/>
-    <col min="1496" max="1733" width="9.06640625" style="8"/>
-    <col min="1734" max="1734" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="1735" max="1735" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1736" max="1736" width="10.59765625" style="8" customWidth="1"/>
-    <col min="1737" max="1751" width="10.73046875" style="8" customWidth="1"/>
-    <col min="1752" max="1989" width="9.06640625" style="8"/>
-    <col min="1990" max="1990" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="1991" max="1991" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1992" max="1992" width="10.59765625" style="8" customWidth="1"/>
-    <col min="1993" max="2007" width="10.73046875" style="8" customWidth="1"/>
-    <col min="2008" max="2245" width="9.06640625" style="8"/>
-    <col min="2246" max="2246" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2247" max="2247" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2248" max="2248" width="10.59765625" style="8" customWidth="1"/>
-    <col min="2249" max="2263" width="10.73046875" style="8" customWidth="1"/>
-    <col min="2264" max="2501" width="9.06640625" style="8"/>
-    <col min="2502" max="2502" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2503" max="2503" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2504" max="2504" width="10.59765625" style="8" customWidth="1"/>
-    <col min="2505" max="2519" width="10.73046875" style="8" customWidth="1"/>
-    <col min="2520" max="2757" width="9.06640625" style="8"/>
-    <col min="2758" max="2758" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2759" max="2759" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2760" max="2760" width="10.59765625" style="8" customWidth="1"/>
-    <col min="2761" max="2775" width="10.73046875" style="8" customWidth="1"/>
-    <col min="2776" max="3013" width="9.06640625" style="8"/>
-    <col min="3014" max="3014" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3015" max="3015" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3016" max="3016" width="10.59765625" style="8" customWidth="1"/>
-    <col min="3017" max="3031" width="10.73046875" style="8" customWidth="1"/>
-    <col min="3032" max="3269" width="9.06640625" style="8"/>
-    <col min="3270" max="3270" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3271" max="3271" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3272" max="3272" width="10.59765625" style="8" customWidth="1"/>
-    <col min="3273" max="3287" width="10.73046875" style="8" customWidth="1"/>
-    <col min="3288" max="3525" width="9.06640625" style="8"/>
-    <col min="3526" max="3526" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3527" max="3527" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3528" max="3528" width="10.59765625" style="8" customWidth="1"/>
-    <col min="3529" max="3543" width="10.73046875" style="8" customWidth="1"/>
-    <col min="3544" max="3781" width="9.06640625" style="8"/>
-    <col min="3782" max="3782" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3783" max="3783" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3784" max="3784" width="10.59765625" style="8" customWidth="1"/>
-    <col min="3785" max="3799" width="10.73046875" style="8" customWidth="1"/>
-    <col min="3800" max="4037" width="9.06640625" style="8"/>
-    <col min="4038" max="4038" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4039" max="4039" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4040" max="4040" width="10.59765625" style="8" customWidth="1"/>
-    <col min="4041" max="4055" width="10.73046875" style="8" customWidth="1"/>
-    <col min="4056" max="4293" width="9.06640625" style="8"/>
-    <col min="4294" max="4294" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4295" max="4295" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4296" max="4296" width="10.59765625" style="8" customWidth="1"/>
-    <col min="4297" max="4311" width="10.73046875" style="8" customWidth="1"/>
-    <col min="4312" max="4549" width="9.06640625" style="8"/>
-    <col min="4550" max="4550" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4551" max="4551" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4552" max="4552" width="10.59765625" style="8" customWidth="1"/>
-    <col min="4553" max="4567" width="10.73046875" style="8" customWidth="1"/>
-    <col min="4568" max="4805" width="9.06640625" style="8"/>
-    <col min="4806" max="4806" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4807" max="4807" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4808" max="4808" width="10.59765625" style="8" customWidth="1"/>
-    <col min="4809" max="4823" width="10.73046875" style="8" customWidth="1"/>
-    <col min="4824" max="5061" width="9.06640625" style="8"/>
-    <col min="5062" max="5062" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5063" max="5063" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5064" max="5064" width="10.59765625" style="8" customWidth="1"/>
-    <col min="5065" max="5079" width="10.73046875" style="8" customWidth="1"/>
-    <col min="5080" max="5317" width="9.06640625" style="8"/>
-    <col min="5318" max="5318" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5319" max="5319" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5320" max="5320" width="10.59765625" style="8" customWidth="1"/>
-    <col min="5321" max="5335" width="10.73046875" style="8" customWidth="1"/>
-    <col min="5336" max="5573" width="9.06640625" style="8"/>
-    <col min="5574" max="5574" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5575" max="5575" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5576" max="5576" width="10.59765625" style="8" customWidth="1"/>
-    <col min="5577" max="5591" width="10.73046875" style="8" customWidth="1"/>
-    <col min="5592" max="5829" width="9.06640625" style="8"/>
-    <col min="5830" max="5830" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5831" max="5831" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5832" max="5832" width="10.59765625" style="8" customWidth="1"/>
-    <col min="5833" max="5847" width="10.73046875" style="8" customWidth="1"/>
-    <col min="5848" max="6085" width="9.06640625" style="8"/>
-    <col min="6086" max="6086" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6087" max="6087" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6088" max="6088" width="10.59765625" style="8" customWidth="1"/>
-    <col min="6089" max="6103" width="10.73046875" style="8" customWidth="1"/>
-    <col min="6104" max="6341" width="9.06640625" style="8"/>
-    <col min="6342" max="6342" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6343" max="6343" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6344" max="6344" width="10.59765625" style="8" customWidth="1"/>
-    <col min="6345" max="6359" width="10.73046875" style="8" customWidth="1"/>
-    <col min="6360" max="6597" width="9.06640625" style="8"/>
-    <col min="6598" max="6598" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6599" max="6599" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6600" max="6600" width="10.59765625" style="8" customWidth="1"/>
-    <col min="6601" max="6615" width="10.73046875" style="8" customWidth="1"/>
-    <col min="6616" max="6853" width="9.06640625" style="8"/>
-    <col min="6854" max="6854" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6855" max="6855" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6856" max="6856" width="10.59765625" style="8" customWidth="1"/>
-    <col min="6857" max="6871" width="10.73046875" style="8" customWidth="1"/>
-    <col min="6872" max="7109" width="9.06640625" style="8"/>
-    <col min="7110" max="7110" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7111" max="7111" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7112" max="7112" width="10.59765625" style="8" customWidth="1"/>
-    <col min="7113" max="7127" width="10.73046875" style="8" customWidth="1"/>
-    <col min="7128" max="7365" width="9.06640625" style="8"/>
-    <col min="7366" max="7366" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7367" max="7367" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7368" max="7368" width="10.59765625" style="8" customWidth="1"/>
-    <col min="7369" max="7383" width="10.73046875" style="8" customWidth="1"/>
-    <col min="7384" max="7621" width="9.06640625" style="8"/>
-    <col min="7622" max="7622" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7623" max="7623" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7624" max="7624" width="10.59765625" style="8" customWidth="1"/>
-    <col min="7625" max="7639" width="10.73046875" style="8" customWidth="1"/>
-    <col min="7640" max="7877" width="9.06640625" style="8"/>
-    <col min="7878" max="7878" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7879" max="7879" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7880" max="7880" width="10.59765625" style="8" customWidth="1"/>
-    <col min="7881" max="7895" width="10.73046875" style="8" customWidth="1"/>
-    <col min="7896" max="8133" width="9.06640625" style="8"/>
-    <col min="8134" max="8134" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8135" max="8135" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8136" max="8136" width="10.59765625" style="8" customWidth="1"/>
-    <col min="8137" max="8151" width="10.73046875" style="8" customWidth="1"/>
-    <col min="8152" max="8389" width="9.06640625" style="8"/>
-    <col min="8390" max="8390" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8391" max="8391" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8392" max="8392" width="10.59765625" style="8" customWidth="1"/>
-    <col min="8393" max="8407" width="10.73046875" style="8" customWidth="1"/>
-    <col min="8408" max="8645" width="9.06640625" style="8"/>
-    <col min="8646" max="8646" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8647" max="8647" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8648" max="8648" width="10.59765625" style="8" customWidth="1"/>
-    <col min="8649" max="8663" width="10.73046875" style="8" customWidth="1"/>
-    <col min="8664" max="8901" width="9.06640625" style="8"/>
-    <col min="8902" max="8902" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8903" max="8903" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8904" max="8904" width="10.59765625" style="8" customWidth="1"/>
-    <col min="8905" max="8919" width="10.73046875" style="8" customWidth="1"/>
-    <col min="8920" max="9157" width="9.06640625" style="8"/>
-    <col min="9158" max="9158" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9159" max="9159" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9160" max="9160" width="10.59765625" style="8" customWidth="1"/>
-    <col min="9161" max="9175" width="10.73046875" style="8" customWidth="1"/>
-    <col min="9176" max="9413" width="9.06640625" style="8"/>
-    <col min="9414" max="9414" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9415" max="9415" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9416" max="9416" width="10.59765625" style="8" customWidth="1"/>
-    <col min="9417" max="9431" width="10.73046875" style="8" customWidth="1"/>
-    <col min="9432" max="9669" width="9.06640625" style="8"/>
-    <col min="9670" max="9670" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9671" max="9671" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9672" max="9672" width="10.59765625" style="8" customWidth="1"/>
-    <col min="9673" max="9687" width="10.73046875" style="8" customWidth="1"/>
-    <col min="9688" max="9925" width="9.06640625" style="8"/>
-    <col min="9926" max="9926" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9927" max="9927" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9928" max="9928" width="10.59765625" style="8" customWidth="1"/>
-    <col min="9929" max="9943" width="10.73046875" style="8" customWidth="1"/>
-    <col min="9944" max="10181" width="9.06640625" style="8"/>
-    <col min="10182" max="10182" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10183" max="10183" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10184" max="10184" width="10.59765625" style="8" customWidth="1"/>
-    <col min="10185" max="10199" width="10.73046875" style="8" customWidth="1"/>
-    <col min="10200" max="10437" width="9.06640625" style="8"/>
-    <col min="10438" max="10438" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10439" max="10439" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10440" max="10440" width="10.59765625" style="8" customWidth="1"/>
-    <col min="10441" max="10455" width="10.73046875" style="8" customWidth="1"/>
-    <col min="10456" max="10693" width="9.06640625" style="8"/>
-    <col min="10694" max="10694" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10695" max="10695" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10696" max="10696" width="10.59765625" style="8" customWidth="1"/>
-    <col min="10697" max="10711" width="10.73046875" style="8" customWidth="1"/>
-    <col min="10712" max="10949" width="9.06640625" style="8"/>
-    <col min="10950" max="10950" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10951" max="10951" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10952" max="10952" width="10.59765625" style="8" customWidth="1"/>
-    <col min="10953" max="10967" width="10.73046875" style="8" customWidth="1"/>
-    <col min="10968" max="11205" width="9.06640625" style="8"/>
-    <col min="11206" max="11206" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11207" max="11207" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11208" max="11208" width="10.59765625" style="8" customWidth="1"/>
-    <col min="11209" max="11223" width="10.73046875" style="8" customWidth="1"/>
-    <col min="11224" max="11461" width="9.06640625" style="8"/>
-    <col min="11462" max="11462" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11463" max="11463" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11464" max="11464" width="10.59765625" style="8" customWidth="1"/>
-    <col min="11465" max="11479" width="10.73046875" style="8" customWidth="1"/>
-    <col min="11480" max="11717" width="9.06640625" style="8"/>
-    <col min="11718" max="11718" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11719" max="11719" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11720" max="11720" width="10.59765625" style="8" customWidth="1"/>
-    <col min="11721" max="11735" width="10.73046875" style="8" customWidth="1"/>
-    <col min="11736" max="11973" width="9.06640625" style="8"/>
-    <col min="11974" max="11974" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11975" max="11975" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11976" max="11976" width="10.59765625" style="8" customWidth="1"/>
-    <col min="11977" max="11991" width="10.73046875" style="8" customWidth="1"/>
-    <col min="11992" max="12229" width="9.06640625" style="8"/>
-    <col min="12230" max="12230" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12231" max="12231" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12232" max="12232" width="10.59765625" style="8" customWidth="1"/>
-    <col min="12233" max="12247" width="10.73046875" style="8" customWidth="1"/>
-    <col min="12248" max="12485" width="9.06640625" style="8"/>
-    <col min="12486" max="12486" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12487" max="12487" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12488" max="12488" width="10.59765625" style="8" customWidth="1"/>
-    <col min="12489" max="12503" width="10.73046875" style="8" customWidth="1"/>
-    <col min="12504" max="12741" width="9.06640625" style="8"/>
-    <col min="12742" max="12742" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12743" max="12743" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12744" max="12744" width="10.59765625" style="8" customWidth="1"/>
-    <col min="12745" max="12759" width="10.73046875" style="8" customWidth="1"/>
-    <col min="12760" max="12997" width="9.06640625" style="8"/>
-    <col min="12998" max="12998" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12999" max="12999" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13000" max="13000" width="10.59765625" style="8" customWidth="1"/>
-    <col min="13001" max="13015" width="10.73046875" style="8" customWidth="1"/>
-    <col min="13016" max="13253" width="9.06640625" style="8"/>
-    <col min="13254" max="13254" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13255" max="13255" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13256" max="13256" width="10.59765625" style="8" customWidth="1"/>
-    <col min="13257" max="13271" width="10.73046875" style="8" customWidth="1"/>
-    <col min="13272" max="13509" width="9.06640625" style="8"/>
-    <col min="13510" max="13510" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13511" max="13511" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13512" max="13512" width="10.59765625" style="8" customWidth="1"/>
-    <col min="13513" max="13527" width="10.73046875" style="8" customWidth="1"/>
-    <col min="13528" max="13765" width="9.06640625" style="8"/>
-    <col min="13766" max="13766" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13767" max="13767" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13768" max="13768" width="10.59765625" style="8" customWidth="1"/>
-    <col min="13769" max="13783" width="10.73046875" style="8" customWidth="1"/>
-    <col min="13784" max="14021" width="9.06640625" style="8"/>
-    <col min="14022" max="14022" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14023" max="14023" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14024" max="14024" width="10.59765625" style="8" customWidth="1"/>
-    <col min="14025" max="14039" width="10.73046875" style="8" customWidth="1"/>
-    <col min="14040" max="14277" width="9.06640625" style="8"/>
-    <col min="14278" max="14278" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14279" max="14279" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14280" max="14280" width="10.59765625" style="8" customWidth="1"/>
-    <col min="14281" max="14295" width="10.73046875" style="8" customWidth="1"/>
-    <col min="14296" max="14533" width="9.06640625" style="8"/>
-    <col min="14534" max="14534" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14535" max="14535" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14536" max="14536" width="10.59765625" style="8" customWidth="1"/>
-    <col min="14537" max="14551" width="10.73046875" style="8" customWidth="1"/>
-    <col min="14552" max="14789" width="9.06640625" style="8"/>
-    <col min="14790" max="14790" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14791" max="14791" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14792" max="14792" width="10.59765625" style="8" customWidth="1"/>
-    <col min="14793" max="14807" width="10.73046875" style="8" customWidth="1"/>
-    <col min="14808" max="15045" width="9.06640625" style="8"/>
-    <col min="15046" max="15046" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15047" max="15047" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15048" max="15048" width="10.59765625" style="8" customWidth="1"/>
-    <col min="15049" max="15063" width="10.73046875" style="8" customWidth="1"/>
-    <col min="15064" max="15301" width="9.06640625" style="8"/>
-    <col min="15302" max="15302" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15303" max="15303" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15304" max="15304" width="10.59765625" style="8" customWidth="1"/>
-    <col min="15305" max="15319" width="10.73046875" style="8" customWidth="1"/>
-    <col min="15320" max="15557" width="9.06640625" style="8"/>
-    <col min="15558" max="15558" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15559" max="15559" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15560" max="15560" width="10.59765625" style="8" customWidth="1"/>
-    <col min="15561" max="15575" width="10.73046875" style="8" customWidth="1"/>
-    <col min="15576" max="15813" width="9.06640625" style="8"/>
-    <col min="15814" max="15814" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15815" max="15815" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15816" max="15816" width="10.59765625" style="8" customWidth="1"/>
-    <col min="15817" max="15831" width="10.73046875" style="8" customWidth="1"/>
-    <col min="15832" max="16069" width="9.06640625" style="8"/>
-    <col min="16070" max="16070" width="21.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16071" max="16071" width="19.265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16072" max="16072" width="10.59765625" style="8" customWidth="1"/>
-    <col min="16073" max="16087" width="10.73046875" style="8" customWidth="1"/>
-    <col min="16088" max="16384" width="9.06640625" style="8"/>
+    <col min="1" max="1" width="32.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" style="8"/>
+    <col min="3" max="3" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" style="27" customWidth="1"/>
+    <col min="6" max="7" width="15.6328125" style="8" customWidth="1"/>
+    <col min="8" max="9" width="10.7265625" style="9" customWidth="1"/>
+    <col min="10" max="197" width="9.08984375" style="8"/>
+    <col min="198" max="198" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="10.6328125" style="8" customWidth="1"/>
+    <col min="201" max="215" width="10.7265625" style="8" customWidth="1"/>
+    <col min="216" max="453" width="9.08984375" style="8"/>
+    <col min="454" max="454" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="455" max="455" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="456" max="456" width="10.6328125" style="8" customWidth="1"/>
+    <col min="457" max="471" width="10.7265625" style="8" customWidth="1"/>
+    <col min="472" max="709" width="9.08984375" style="8"/>
+    <col min="710" max="710" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="711" max="711" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="712" max="712" width="10.6328125" style="8" customWidth="1"/>
+    <col min="713" max="727" width="10.7265625" style="8" customWidth="1"/>
+    <col min="728" max="965" width="9.08984375" style="8"/>
+    <col min="966" max="966" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="967" max="967" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="968" max="968" width="10.6328125" style="8" customWidth="1"/>
+    <col min="969" max="983" width="10.7265625" style="8" customWidth="1"/>
+    <col min="984" max="1221" width="9.08984375" style="8"/>
+    <col min="1222" max="1222" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1223" max="1223" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1224" max="1224" width="10.6328125" style="8" customWidth="1"/>
+    <col min="1225" max="1239" width="10.7265625" style="8" customWidth="1"/>
+    <col min="1240" max="1477" width="9.08984375" style="8"/>
+    <col min="1478" max="1478" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1479" max="1479" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1480" max="1480" width="10.6328125" style="8" customWidth="1"/>
+    <col min="1481" max="1495" width="10.7265625" style="8" customWidth="1"/>
+    <col min="1496" max="1733" width="9.08984375" style="8"/>
+    <col min="1734" max="1734" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1735" max="1735" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1736" max="1736" width="10.6328125" style="8" customWidth="1"/>
+    <col min="1737" max="1751" width="10.7265625" style="8" customWidth="1"/>
+    <col min="1752" max="1989" width="9.08984375" style="8"/>
+    <col min="1990" max="1990" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1991" max="1991" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1992" max="1992" width="10.6328125" style="8" customWidth="1"/>
+    <col min="1993" max="2007" width="10.7265625" style="8" customWidth="1"/>
+    <col min="2008" max="2245" width="9.08984375" style="8"/>
+    <col min="2246" max="2246" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2247" max="2247" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2248" max="2248" width="10.6328125" style="8" customWidth="1"/>
+    <col min="2249" max="2263" width="10.7265625" style="8" customWidth="1"/>
+    <col min="2264" max="2501" width="9.08984375" style="8"/>
+    <col min="2502" max="2502" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2503" max="2503" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2504" max="2504" width="10.6328125" style="8" customWidth="1"/>
+    <col min="2505" max="2519" width="10.7265625" style="8" customWidth="1"/>
+    <col min="2520" max="2757" width="9.08984375" style="8"/>
+    <col min="2758" max="2758" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2759" max="2759" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2760" max="2760" width="10.6328125" style="8" customWidth="1"/>
+    <col min="2761" max="2775" width="10.7265625" style="8" customWidth="1"/>
+    <col min="2776" max="3013" width="9.08984375" style="8"/>
+    <col min="3014" max="3014" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3015" max="3015" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3016" max="3016" width="10.6328125" style="8" customWidth="1"/>
+    <col min="3017" max="3031" width="10.7265625" style="8" customWidth="1"/>
+    <col min="3032" max="3269" width="9.08984375" style="8"/>
+    <col min="3270" max="3270" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3271" max="3271" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3272" max="3272" width="10.6328125" style="8" customWidth="1"/>
+    <col min="3273" max="3287" width="10.7265625" style="8" customWidth="1"/>
+    <col min="3288" max="3525" width="9.08984375" style="8"/>
+    <col min="3526" max="3526" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3527" max="3527" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3528" max="3528" width="10.6328125" style="8" customWidth="1"/>
+    <col min="3529" max="3543" width="10.7265625" style="8" customWidth="1"/>
+    <col min="3544" max="3781" width="9.08984375" style="8"/>
+    <col min="3782" max="3782" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3783" max="3783" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3784" max="3784" width="10.6328125" style="8" customWidth="1"/>
+    <col min="3785" max="3799" width="10.7265625" style="8" customWidth="1"/>
+    <col min="3800" max="4037" width="9.08984375" style="8"/>
+    <col min="4038" max="4038" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4039" max="4039" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4040" max="4040" width="10.6328125" style="8" customWidth="1"/>
+    <col min="4041" max="4055" width="10.7265625" style="8" customWidth="1"/>
+    <col min="4056" max="4293" width="9.08984375" style="8"/>
+    <col min="4294" max="4294" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4295" max="4295" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4296" max="4296" width="10.6328125" style="8" customWidth="1"/>
+    <col min="4297" max="4311" width="10.7265625" style="8" customWidth="1"/>
+    <col min="4312" max="4549" width="9.08984375" style="8"/>
+    <col min="4550" max="4550" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4551" max="4551" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4552" max="4552" width="10.6328125" style="8" customWidth="1"/>
+    <col min="4553" max="4567" width="10.7265625" style="8" customWidth="1"/>
+    <col min="4568" max="4805" width="9.08984375" style="8"/>
+    <col min="4806" max="4806" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4807" max="4807" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4808" max="4808" width="10.6328125" style="8" customWidth="1"/>
+    <col min="4809" max="4823" width="10.7265625" style="8" customWidth="1"/>
+    <col min="4824" max="5061" width="9.08984375" style="8"/>
+    <col min="5062" max="5062" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5063" max="5063" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5064" max="5064" width="10.6328125" style="8" customWidth="1"/>
+    <col min="5065" max="5079" width="10.7265625" style="8" customWidth="1"/>
+    <col min="5080" max="5317" width="9.08984375" style="8"/>
+    <col min="5318" max="5318" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5319" max="5319" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5320" max="5320" width="10.6328125" style="8" customWidth="1"/>
+    <col min="5321" max="5335" width="10.7265625" style="8" customWidth="1"/>
+    <col min="5336" max="5573" width="9.08984375" style="8"/>
+    <col min="5574" max="5574" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5575" max="5575" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5576" max="5576" width="10.6328125" style="8" customWidth="1"/>
+    <col min="5577" max="5591" width="10.7265625" style="8" customWidth="1"/>
+    <col min="5592" max="5829" width="9.08984375" style="8"/>
+    <col min="5830" max="5830" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5831" max="5831" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5832" max="5832" width="10.6328125" style="8" customWidth="1"/>
+    <col min="5833" max="5847" width="10.7265625" style="8" customWidth="1"/>
+    <col min="5848" max="6085" width="9.08984375" style="8"/>
+    <col min="6086" max="6086" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6087" max="6087" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6088" max="6088" width="10.6328125" style="8" customWidth="1"/>
+    <col min="6089" max="6103" width="10.7265625" style="8" customWidth="1"/>
+    <col min="6104" max="6341" width="9.08984375" style="8"/>
+    <col min="6342" max="6342" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6343" max="6343" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6344" max="6344" width="10.6328125" style="8" customWidth="1"/>
+    <col min="6345" max="6359" width="10.7265625" style="8" customWidth="1"/>
+    <col min="6360" max="6597" width="9.08984375" style="8"/>
+    <col min="6598" max="6598" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6599" max="6599" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6600" max="6600" width="10.6328125" style="8" customWidth="1"/>
+    <col min="6601" max="6615" width="10.7265625" style="8" customWidth="1"/>
+    <col min="6616" max="6853" width="9.08984375" style="8"/>
+    <col min="6854" max="6854" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6855" max="6855" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6856" max="6856" width="10.6328125" style="8" customWidth="1"/>
+    <col min="6857" max="6871" width="10.7265625" style="8" customWidth="1"/>
+    <col min="6872" max="7109" width="9.08984375" style="8"/>
+    <col min="7110" max="7110" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7111" max="7111" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7112" max="7112" width="10.6328125" style="8" customWidth="1"/>
+    <col min="7113" max="7127" width="10.7265625" style="8" customWidth="1"/>
+    <col min="7128" max="7365" width="9.08984375" style="8"/>
+    <col min="7366" max="7366" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7367" max="7367" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7368" max="7368" width="10.6328125" style="8" customWidth="1"/>
+    <col min="7369" max="7383" width="10.7265625" style="8" customWidth="1"/>
+    <col min="7384" max="7621" width="9.08984375" style="8"/>
+    <col min="7622" max="7622" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7623" max="7623" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7624" max="7624" width="10.6328125" style="8" customWidth="1"/>
+    <col min="7625" max="7639" width="10.7265625" style="8" customWidth="1"/>
+    <col min="7640" max="7877" width="9.08984375" style="8"/>
+    <col min="7878" max="7878" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7879" max="7879" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7880" max="7880" width="10.6328125" style="8" customWidth="1"/>
+    <col min="7881" max="7895" width="10.7265625" style="8" customWidth="1"/>
+    <col min="7896" max="8133" width="9.08984375" style="8"/>
+    <col min="8134" max="8134" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8135" max="8135" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8136" max="8136" width="10.6328125" style="8" customWidth="1"/>
+    <col min="8137" max="8151" width="10.7265625" style="8" customWidth="1"/>
+    <col min="8152" max="8389" width="9.08984375" style="8"/>
+    <col min="8390" max="8390" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8391" max="8391" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8392" max="8392" width="10.6328125" style="8" customWidth="1"/>
+    <col min="8393" max="8407" width="10.7265625" style="8" customWidth="1"/>
+    <col min="8408" max="8645" width="9.08984375" style="8"/>
+    <col min="8646" max="8646" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8647" max="8647" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8648" max="8648" width="10.6328125" style="8" customWidth="1"/>
+    <col min="8649" max="8663" width="10.7265625" style="8" customWidth="1"/>
+    <col min="8664" max="8901" width="9.08984375" style="8"/>
+    <col min="8902" max="8902" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8903" max="8903" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8904" max="8904" width="10.6328125" style="8" customWidth="1"/>
+    <col min="8905" max="8919" width="10.7265625" style="8" customWidth="1"/>
+    <col min="8920" max="9157" width="9.08984375" style="8"/>
+    <col min="9158" max="9158" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9159" max="9159" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9160" max="9160" width="10.6328125" style="8" customWidth="1"/>
+    <col min="9161" max="9175" width="10.7265625" style="8" customWidth="1"/>
+    <col min="9176" max="9413" width="9.08984375" style="8"/>
+    <col min="9414" max="9414" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9415" max="9415" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9416" max="9416" width="10.6328125" style="8" customWidth="1"/>
+    <col min="9417" max="9431" width="10.7265625" style="8" customWidth="1"/>
+    <col min="9432" max="9669" width="9.08984375" style="8"/>
+    <col min="9670" max="9670" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9671" max="9671" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9672" max="9672" width="10.6328125" style="8" customWidth="1"/>
+    <col min="9673" max="9687" width="10.7265625" style="8" customWidth="1"/>
+    <col min="9688" max="9925" width="9.08984375" style="8"/>
+    <col min="9926" max="9926" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9927" max="9927" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9928" max="9928" width="10.6328125" style="8" customWidth="1"/>
+    <col min="9929" max="9943" width="10.7265625" style="8" customWidth="1"/>
+    <col min="9944" max="10181" width="9.08984375" style="8"/>
+    <col min="10182" max="10182" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="10183" max="10183" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10184" max="10184" width="10.6328125" style="8" customWidth="1"/>
+    <col min="10185" max="10199" width="10.7265625" style="8" customWidth="1"/>
+    <col min="10200" max="10437" width="9.08984375" style="8"/>
+    <col min="10438" max="10438" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="10439" max="10439" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10440" max="10440" width="10.6328125" style="8" customWidth="1"/>
+    <col min="10441" max="10455" width="10.7265625" style="8" customWidth="1"/>
+    <col min="10456" max="10693" width="9.08984375" style="8"/>
+    <col min="10694" max="10694" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="10695" max="10695" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10696" max="10696" width="10.6328125" style="8" customWidth="1"/>
+    <col min="10697" max="10711" width="10.7265625" style="8" customWidth="1"/>
+    <col min="10712" max="10949" width="9.08984375" style="8"/>
+    <col min="10950" max="10950" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="10951" max="10951" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10952" max="10952" width="10.6328125" style="8" customWidth="1"/>
+    <col min="10953" max="10967" width="10.7265625" style="8" customWidth="1"/>
+    <col min="10968" max="11205" width="9.08984375" style="8"/>
+    <col min="11206" max="11206" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11207" max="11207" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11208" max="11208" width="10.6328125" style="8" customWidth="1"/>
+    <col min="11209" max="11223" width="10.7265625" style="8" customWidth="1"/>
+    <col min="11224" max="11461" width="9.08984375" style="8"/>
+    <col min="11462" max="11462" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11463" max="11463" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11464" max="11464" width="10.6328125" style="8" customWidth="1"/>
+    <col min="11465" max="11479" width="10.7265625" style="8" customWidth="1"/>
+    <col min="11480" max="11717" width="9.08984375" style="8"/>
+    <col min="11718" max="11718" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11719" max="11719" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11720" max="11720" width="10.6328125" style="8" customWidth="1"/>
+    <col min="11721" max="11735" width="10.7265625" style="8" customWidth="1"/>
+    <col min="11736" max="11973" width="9.08984375" style="8"/>
+    <col min="11974" max="11974" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11975" max="11975" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11976" max="11976" width="10.6328125" style="8" customWidth="1"/>
+    <col min="11977" max="11991" width="10.7265625" style="8" customWidth="1"/>
+    <col min="11992" max="12229" width="9.08984375" style="8"/>
+    <col min="12230" max="12230" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12231" max="12231" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12232" max="12232" width="10.6328125" style="8" customWidth="1"/>
+    <col min="12233" max="12247" width="10.7265625" style="8" customWidth="1"/>
+    <col min="12248" max="12485" width="9.08984375" style="8"/>
+    <col min="12486" max="12486" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12487" max="12487" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12488" max="12488" width="10.6328125" style="8" customWidth="1"/>
+    <col min="12489" max="12503" width="10.7265625" style="8" customWidth="1"/>
+    <col min="12504" max="12741" width="9.08984375" style="8"/>
+    <col min="12742" max="12742" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12743" max="12743" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12744" max="12744" width="10.6328125" style="8" customWidth="1"/>
+    <col min="12745" max="12759" width="10.7265625" style="8" customWidth="1"/>
+    <col min="12760" max="12997" width="9.08984375" style="8"/>
+    <col min="12998" max="12998" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12999" max="12999" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13000" max="13000" width="10.6328125" style="8" customWidth="1"/>
+    <col min="13001" max="13015" width="10.7265625" style="8" customWidth="1"/>
+    <col min="13016" max="13253" width="9.08984375" style="8"/>
+    <col min="13254" max="13254" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="13255" max="13255" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13256" max="13256" width="10.6328125" style="8" customWidth="1"/>
+    <col min="13257" max="13271" width="10.7265625" style="8" customWidth="1"/>
+    <col min="13272" max="13509" width="9.08984375" style="8"/>
+    <col min="13510" max="13510" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="13511" max="13511" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13512" max="13512" width="10.6328125" style="8" customWidth="1"/>
+    <col min="13513" max="13527" width="10.7265625" style="8" customWidth="1"/>
+    <col min="13528" max="13765" width="9.08984375" style="8"/>
+    <col min="13766" max="13766" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="13767" max="13767" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13768" max="13768" width="10.6328125" style="8" customWidth="1"/>
+    <col min="13769" max="13783" width="10.7265625" style="8" customWidth="1"/>
+    <col min="13784" max="14021" width="9.08984375" style="8"/>
+    <col min="14022" max="14022" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="14023" max="14023" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14024" max="14024" width="10.6328125" style="8" customWidth="1"/>
+    <col min="14025" max="14039" width="10.7265625" style="8" customWidth="1"/>
+    <col min="14040" max="14277" width="9.08984375" style="8"/>
+    <col min="14278" max="14278" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="14279" max="14279" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14280" max="14280" width="10.6328125" style="8" customWidth="1"/>
+    <col min="14281" max="14295" width="10.7265625" style="8" customWidth="1"/>
+    <col min="14296" max="14533" width="9.08984375" style="8"/>
+    <col min="14534" max="14534" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="14535" max="14535" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14536" max="14536" width="10.6328125" style="8" customWidth="1"/>
+    <col min="14537" max="14551" width="10.7265625" style="8" customWidth="1"/>
+    <col min="14552" max="14789" width="9.08984375" style="8"/>
+    <col min="14790" max="14790" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="14791" max="14791" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14792" max="14792" width="10.6328125" style="8" customWidth="1"/>
+    <col min="14793" max="14807" width="10.7265625" style="8" customWidth="1"/>
+    <col min="14808" max="15045" width="9.08984375" style="8"/>
+    <col min="15046" max="15046" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15047" max="15047" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15048" max="15048" width="10.6328125" style="8" customWidth="1"/>
+    <col min="15049" max="15063" width="10.7265625" style="8" customWidth="1"/>
+    <col min="15064" max="15301" width="9.08984375" style="8"/>
+    <col min="15302" max="15302" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15303" max="15303" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15304" max="15304" width="10.6328125" style="8" customWidth="1"/>
+    <col min="15305" max="15319" width="10.7265625" style="8" customWidth="1"/>
+    <col min="15320" max="15557" width="9.08984375" style="8"/>
+    <col min="15558" max="15558" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15559" max="15559" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15560" max="15560" width="10.6328125" style="8" customWidth="1"/>
+    <col min="15561" max="15575" width="10.7265625" style="8" customWidth="1"/>
+    <col min="15576" max="15813" width="9.08984375" style="8"/>
+    <col min="15814" max="15814" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15815" max="15815" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15816" max="15816" width="10.6328125" style="8" customWidth="1"/>
+    <col min="15817" max="15831" width="10.7265625" style="8" customWidth="1"/>
+    <col min="15832" max="16069" width="9.08984375" style="8"/>
+    <col min="16070" max="16070" width="21.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="16071" max="16071" width="19.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16072" max="16072" width="10.6328125" style="8" customWidth="1"/>
+    <col min="16073" max="16087" width="10.7265625" style="8" customWidth="1"/>
+    <col min="16088" max="16384" width="9.08984375" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="39.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -985,17 +1015,17 @@
       <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>25</v>
@@ -1004,7 +1034,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>0</v>
       </c>
@@ -1014,32 +1044,32 @@
       <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="27">
         <v>326133</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="28">
         <v>0.15532739043525848</v>
       </c>
       <c r="F3">
-        <v>274222</v>
-      </c>
-      <c r="G3" s="42">
+        <v>206368</v>
+      </c>
+      <c r="G3" s="40">
         <f>F3/SUM(F$3:F$13)</f>
-        <v>0.15180799196486278</v>
+        <v>0.11424484296095033</v>
       </c>
       <c r="H3" s="10">
         <f ca="1">INDIRECT("'[carown_summary.csv]carown_summary'!b2")</f>
-        <v>280798</v>
+        <v>207561</v>
       </c>
       <c r="I3" s="1">
         <f ca="1">H3/H$16</f>
-        <v>0.15544842873070583</v>
+        <v>0.11490528497547009</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>0</v>
       </c>
@@ -1049,32 +1079,32 @@
       <c r="C4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="27">
         <v>366889.55612416414</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="28">
         <v>0.17473851873535251</v>
       </c>
       <c r="F4">
-        <v>507083.59399999998</v>
-      </c>
-      <c r="G4" s="42">
+        <v>570250</v>
+      </c>
+      <c r="G4" s="40">
         <f t="shared" ref="G4:G13" si="0">F4/SUM(F$3:F$13)</f>
-        <v>0.28071906033602606</v>
+        <v>0.31568906854978446</v>
       </c>
       <c r="H4" s="10">
         <f ca="1">INDIRECT("'[carown_summary.csv]carown_summary'!b3")</f>
-        <v>488477</v>
+        <v>545103</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" ref="I4:I13" ca="1" si="1">H4/H$16</f>
-        <v>0.27041852905323038</v>
+        <v>0.30176774806434575</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -1084,29 +1114,29 @@
       <c r="C5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="27">
         <v>281798.69522683602</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="28">
         <v>0.13421228749511752</v>
       </c>
       <c r="F5">
-        <v>10311.780000000001</v>
-      </c>
-      <c r="G5" s="42">
+        <v>0</v>
+      </c>
+      <c r="G5" s="40">
         <f t="shared" si="0"/>
-        <v>5.7085522510354116E-3</v>
+        <v>0</v>
       </c>
       <c r="H5" s="10">
         <f ca="1">INDIRECT("'[carown_summary.csv]carown_summary'!b4")</f>
-        <v>10384</v>
+        <v>11075</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7485326958868982E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+        <v>6.1310941414973487E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <v>0</v>
       </c>
@@ -1116,32 +1146,32 @@
       <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="27">
         <v>358998.98199425329</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="28">
         <v>0.17098047435273861</v>
       </c>
       <c r="F6">
-        <v>563901.8770518722</v>
-      </c>
-      <c r="G6" s="42">
+        <v>660103</v>
+      </c>
+      <c r="G6" s="40">
         <f t="shared" si="0"/>
-        <v>0.31217339097687874</v>
+        <v>0.36543147955619182</v>
       </c>
       <c r="H6" s="10">
         <f ca="1">INDIRECT("'[carown_summary.csv]carown_summary'!b5")</f>
-        <v>579626</v>
+        <v>593282</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3208781791589117</v>
+        <v>0.32843952997343839</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -1151,32 +1181,32 @@
       <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="27">
         <v>149034.0819942533</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="28">
         <v>7.0980474352738618E-2</v>
       </c>
       <c r="F7">
-        <v>12949.220000000001</v>
-      </c>
-      <c r="G7" s="42">
+        <v>0</v>
+      </c>
+      <c r="G7" s="40">
         <f t="shared" si="0"/>
-        <v>7.1686264621775072E-3</v>
+        <v>0</v>
       </c>
       <c r="H7" s="10">
         <f ca="1">INDIRECT("'[carown_summary.csv]carown_summary'!b6")</f>
-        <v>13045</v>
+        <v>13105</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2216495587292557E-3</v>
+        <v>7.2548974017447188E-3</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>1</v>
       </c>
@@ -1186,29 +1216,29 @@
       <c r="C8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="27">
         <v>212023.55199425327</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="28">
         <v>0.10098047435273862</v>
       </c>
       <c r="F8">
-        <v>68803.528948127961</v>
-      </c>
-      <c r="G8" s="42">
+        <v>0</v>
+      </c>
+      <c r="G8" s="40">
         <f t="shared" si="0"/>
-        <v>3.8089305634528274E-2</v>
+        <v>0</v>
       </c>
       <c r="H8" s="10">
         <f ca="1">INDIRECT("'[carown_summary.csv]carown_summary'!b7")</f>
-        <v>69288</v>
+        <v>70001</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8357505145667506E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+        <v>3.8752390157919273E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>0</v>
       </c>
@@ -1218,29 +1248,29 @@
       <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="27">
         <v>131670.85453472409</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="28">
         <v>6.2710888598391482E-2</v>
       </c>
       <c r="F9">
-        <v>218451.1702942565</v>
-      </c>
-      <c r="G9" s="42">
+        <v>247817</v>
+      </c>
+      <c r="G9" s="40">
         <f t="shared" si="0"/>
-        <v>0.12093352650314475</v>
+        <v>0.13719091258360708</v>
       </c>
       <c r="H9" s="10">
         <f ca="1">INDIRECT("'[carown_summary.csv]carown_summary'!b8")</f>
-        <v>216287</v>
+        <v>217642</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11973544791942312</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+        <v>0.12048610303781183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>3</v>
       </c>
@@ -1250,29 +1280,29 @@
       <c r="C10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="27">
         <v>44008.260751689981</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="28">
         <v>2.0959817927515494E-2</v>
       </c>
       <c r="F10">
-        <v>6946.4299754930098</v>
-      </c>
-      <c r="G10" s="42">
+        <v>0</v>
+      </c>
+      <c r="G10" s="40">
         <f t="shared" si="0"/>
-        <v>3.8455105203234049E-3</v>
+        <v>0</v>
       </c>
       <c r="H10" s="10">
         <f ca="1">INDIRECT("'[carown_summary.csv]carown_summary'!b9")</f>
-        <v>7060</v>
+        <v>7027</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3.9083822065640889E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+        <v>3.8901307929843673E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>1</v>
       </c>
@@ -1282,29 +1312,29 @@
       <c r="C11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="27">
         <v>47582.372610895975</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="28">
         <v>2.2662060473391494E-2</v>
       </c>
       <c r="F11">
-        <v>15720.55598171567</v>
-      </c>
-      <c r="G11" s="42">
+        <v>0</v>
+      </c>
+      <c r="G11" s="40">
         <f t="shared" si="0"/>
-        <v>8.702824850506042E-3</v>
+        <v>0</v>
       </c>
       <c r="H11" s="10">
         <f ca="1">INDIRECT("'[carown_summary.csv]carown_summary'!b10")</f>
-        <v>15864</v>
+        <v>15703</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7822344652879192E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+        <v>8.6931441357952933E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>2</v>
       </c>
@@ -1314,29 +1344,29 @@
       <c r="C12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="27">
         <v>44008.260751689981</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="28">
         <v>2.0959817927515494E-2</v>
       </c>
       <c r="F12">
-        <v>4920.78</v>
-      </c>
-      <c r="G12" s="42">
+        <v>0</v>
+      </c>
+      <c r="G12" s="40">
         <f t="shared" si="0"/>
-        <v>2.7241203503032482E-3</v>
+        <v>0</v>
       </c>
       <c r="H12" s="10">
         <f ca="1">INDIRECT("'[carown_summary.csv]carown_summary'!b11")</f>
-        <v>4899</v>
+        <v>4939</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7120629504189054E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+        <v>2.7342188681585018E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
         <v>0</v>
       </c>
@@ -1346,139 +1376,139 @@
       <c r="C13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="27">
         <v>137501</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="28">
         <v>6.5487612453319577E-2</v>
       </c>
       <c r="F13">
-        <v>123063</v>
-      </c>
-      <c r="G13" s="42">
+        <v>121828</v>
+      </c>
+      <c r="G13" s="40">
         <f t="shared" si="0"/>
-        <v>6.8127090150213718E-2</v>
+        <v>6.7443696349466273E-2</v>
       </c>
       <c r="H13" s="10">
         <f ca="1">INDIRECT("'[carown_summary.csv]carown_summary'!b12")</f>
-        <v>120646</v>
+        <v>120928</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6.6789048115174374E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="E14" s="30"/>
+        <v>6.6945458450834439E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E14" s="29"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="13"/>
-      <c r="E15" s="31"/>
+      <c r="E15" s="30"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="31">
         <f>SUM(D3:D13)</f>
         <v>2099648.6159827597</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32">
+      <c r="E16" s="30"/>
+      <c r="F16" s="31">
         <f>SUM(F3:F13)</f>
-        <v>1806373.9362514655</v>
+        <v>1806366</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="16">
         <f ca="1">SUM(H3:H13)</f>
-        <v>1806374</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+        <v>1806366</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <f>SUMPRODUCT($B$3:$B$13,D3:D13)</f>
         <v>3495615.1292635193</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32">
+      <c r="E17" s="30"/>
+      <c r="F17" s="31">
         <f>SUMPRODUCT($B$3:$B$13,F3:F13)</f>
-        <v>3088298.634754396</v>
+        <v>3169950.2</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="16">
         <f ca="1">SUMPRODUCT($B$3:$B$13,H3:H13)</f>
-        <v>3085951.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+        <v>3176970.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="31">
         <f>SUMPRODUCT($A$3:$A$13,D3:D13)</f>
         <v>1059514.0875789418</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32">
+      <c r="E18" s="30"/>
+      <c r="F18" s="31">
         <f>SUMPRODUCT($A$3:$A$13,F3:F13)</f>
-        <v>151415.15485632265</v>
+        <v>0</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="16">
         <f ca="1">SUMPRODUCT($A$3:$A$13,H3:H13)</f>
-        <v>152604</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+        <v>153948</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C19" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="32">
         <f>D18/D17</f>
         <v>0.3030980380846926</v>
       </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="33">
+      <c r="E19" s="33"/>
+      <c r="F19" s="32">
         <f>F18/F17</f>
-        <v>4.9028663598902338E-2</v>
+        <v>0</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="3">
         <f ca="1">H18/H17</f>
-        <v>4.9451200041581989E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
+        <v>4.8457489465906854E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C20" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="34">
         <f>D17/D16</f>
         <v>1.6648572064175438</v>
       </c>
-      <c r="F20" s="35">
+      <c r="F20" s="34">
         <f>F17/F16</f>
-        <v>1.7096674020680034</v>
-      </c>
-      <c r="H20" s="45">
+        <v>1.754877029350641</v>
+      </c>
+      <c r="H20" s="43">
         <f ca="1">H17/H16</f>
-        <v>1.7083679238075835</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
+        <v>1.7587632849599695</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="35"/>
+      <c r="E21" s="36"/>
       <c r="H21" s="19"/>
       <c r="I21" s="20"/>
       <c r="K21" s="8"/>
@@ -1490,164 +1520,167 @@
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C22" s="13"/>
-      <c r="D22" s="35"/>
+      <c r="D22" s="34"/>
+      <c r="G22" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="H22" s="2"/>
-      <c r="J22" s="43" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="J22" s="41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="37">
         <f>E3</f>
         <v>0.15532739043525848</v>
       </c>
       <c r="F23" s="21"/>
-      <c r="G23" s="41">
-        <f>G3</f>
-        <v>0.15180799196486278</v>
-      </c>
-      <c r="I23" s="22">
+      <c r="G23" s="45">
+        <v>0.11424484296095033</v>
+      </c>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46">
         <f ca="1">I3</f>
-        <v>0.15544842873070583</v>
-      </c>
-      <c r="J23" s="44">
+        <v>0.11490528497547009</v>
+      </c>
+      <c r="J23" s="42">
         <f ca="1">I23-G23</f>
-        <v>3.6404367658430525E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
+        <v>6.6044201451975759E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="37">
         <f>SUM(E4:E5)</f>
         <v>0.30895080623047</v>
       </c>
       <c r="F24" s="21"/>
-      <c r="G24" s="41">
-        <f>SUM(G4:G5)</f>
-        <v>0.28642761258706145</v>
-      </c>
-      <c r="I24" s="22">
+      <c r="G24" s="45">
+        <v>0.31568906854978446</v>
+      </c>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46">
         <f ca="1">SUM(I4:I5)</f>
-        <v>0.27616706174911726</v>
-      </c>
-      <c r="J24" s="44">
+        <v>0.30789884220584313</v>
+      </c>
+      <c r="J24" s="42">
         <f t="shared" ref="J24:J27" ca="1" si="2">I24-G24</f>
-        <v>-1.0260550837944193E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
+        <v>-7.7902263439413311E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C25" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="37">
         <f>SUM(E6:E8)</f>
         <v>0.34294142305821584</v>
       </c>
       <c r="F25" s="21"/>
-      <c r="G25" s="41">
-        <f>SUM(G6:G8)</f>
-        <v>0.35743132307358455</v>
-      </c>
-      <c r="I25" s="22">
+      <c r="G25" s="45">
+        <v>0.36543147955619182</v>
+      </c>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46">
         <f ca="1">SUM(I6:I8)</f>
-        <v>0.36645733386330848</v>
-      </c>
-      <c r="J25" s="44">
+        <v>0.37444681753310238</v>
+      </c>
+      <c r="J25" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>9.0260107897239261E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
+        <v>9.0153379769105646E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C26" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="38">
+      <c r="E26" s="37">
         <f>SUM(E9:E12)</f>
         <v>0.12729258492681395</v>
       </c>
       <c r="F26" s="21"/>
-      <c r="G26" s="41">
-        <f>SUM(G9:G12)</f>
-        <v>0.13620598222427746</v>
-      </c>
-      <c r="I26" s="22">
+      <c r="G26" s="45">
+        <v>0.13719091258360708</v>
+      </c>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46">
         <f ca="1">SUM(I9:I12)</f>
-        <v>0.13513812754169402</v>
-      </c>
-      <c r="J26" s="44">
+        <v>0.13580359683474999</v>
+      </c>
+      <c r="J26" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>-1.0678546825834412E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
+        <v>-1.3873157488570875E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C27" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="38">
+      <c r="E27" s="37">
         <f>E13</f>
         <v>6.5487612453319577E-2</v>
       </c>
       <c r="F27" s="21"/>
-      <c r="G27" s="41">
-        <f>G13</f>
-        <v>6.8127090150213718E-2</v>
-      </c>
-      <c r="I27" s="22">
+      <c r="G27" s="45">
+        <v>6.7443696349466273E-2</v>
+      </c>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46">
         <f ca="1">I13</f>
-        <v>6.6789048115174374E-2</v>
-      </c>
-      <c r="J27" s="44">
+        <v>6.6945458450834439E-2</v>
+      </c>
+      <c r="J27" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>-1.338042035039344E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
+        <v>-4.9823789863183421E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C30" s="13"/>
-      <c r="D30" s="37"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="D30" s="36"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C31" s="18"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="E32" s="39"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.45">
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.45">
-      <c r="E34" s="40"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E32" s="38"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="E34" s="39"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>